<commit_message>
rimosso file excel + cambiato addressbook in xlsxToArray.mjs
</commit_message>
<xml_diff>
--- a/addressbook/template.xlsx
+++ b/addressbook/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\localSites\Jmailer\addressbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA15F974-09DE-46AD-A808-850BE1B384FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA018D74-671D-4D94-92FB-CDD1800CAFC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4365" yWindow="3975" windowWidth="21600" windowHeight="11505" xr2:uid="{B064F148-654C-4C08-8253-C73EBAFF2FA9}"/>
   </bookViews>
@@ -25,12 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>ADDRESSES</t>
   </si>
   <si>
-    <t>test@domain.com</t>
+    <t>test@domain1.com</t>
+  </si>
+  <si>
+    <t>test@domain2.com</t>
+  </si>
+  <si>
+    <t>test@domain3.com</t>
+  </si>
+  <si>
+    <t>test@domain4.com</t>
+  </si>
+  <si>
+    <t>test@domain5.com</t>
   </si>
 </sst>
 </file>
@@ -400,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6D5E55-2AD3-4FB2-9C3A-CFB2CE9BC6C7}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,6 +433,26 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>